<commit_message>
Developed a running gantry GUI
</commit_message>
<xml_diff>
--- a/Script.xlsx
+++ b/Script.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Alpha Redux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54FE3400-A827-4B94-8864-1960866495F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2455A06A-BFE0-4616-8C39-4BFA383FB26F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2235" yWindow="8250" windowWidth="17280" windowHeight="8925" xr2:uid="{F78622BC-B8A3-4261-86B1-C19D8BE4EB55}"/>
+    <workbookView xWindow="-1875" yWindow="-19200" windowWidth="16530" windowHeight="11340" xr2:uid="{F78622BC-B8A3-4261-86B1-C19D8BE4EB55}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="26">
   <si>
     <t>Step#</t>
   </si>
@@ -78,6 +78,42 @@
   </si>
   <si>
     <t>Wait</t>
+  </si>
+  <si>
+    <t>Parameter3</t>
+  </si>
+  <si>
+    <t>No Parameters</t>
+  </si>
+  <si>
+    <t>Position (mm)</t>
+  </si>
+  <si>
+    <t>Direction (-1/+1)</t>
+  </si>
+  <si>
+    <t>Speed (mm/s)</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>If Speed is 0 it will move at max speed</t>
+  </si>
+  <si>
+    <t>Direction for ABS doesn't matter, leave 0</t>
+  </si>
+  <si>
+    <t>Go To Label</t>
+  </si>
+  <si>
+    <t>Number of times</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Wait (ms)</t>
   </si>
 </sst>
 </file>
@@ -113,8 +149,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,19 +468,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F69CE37-DE2A-400D-95D7-88241DD5D745}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -454,8 +494,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10</v>
       </c>
@@ -468,8 +511,11 @@
       <c r="D2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>20</v>
       </c>
@@ -477,13 +523,16 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>30</v>
       </c>
@@ -491,10 +540,16 @@
         <v>13</v>
       </c>
       <c r="C4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>500</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>40</v>
       </c>
@@ -502,13 +557,16 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>1500</v>
+        <v>300</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>50</v>
       </c>
@@ -518,8 +576,14 @@
       <c r="C6">
         <v>1000</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>60</v>
       </c>
@@ -527,13 +591,16 @@
         <v>8</v>
       </c>
       <c r="C7">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>70</v>
       </c>
@@ -541,10 +608,16 @@
         <v>13</v>
       </c>
       <c r="C8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>500</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>80</v>
       </c>
@@ -552,13 +625,16 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>90</v>
       </c>
@@ -568,8 +644,14 @@
       <c r="C10">
         <v>1000</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>100</v>
       </c>
@@ -580,10 +662,13 @@
         <v>20</v>
       </c>
       <c r="D11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>110</v>
       </c>
@@ -596,18 +681,30 @@
       <c r="D12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>120</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D16" xr:uid="{E060BF54-3F95-4B65-8BA7-AC011ACA6E26}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D11 C13:D16 C12" xr:uid="{E060BF54-3F95-4B65-8BA7-AC011ACA6E26}">
       <formula1>0</formula1>
       <formula2>2000</formula2>
     </dataValidation>
@@ -630,68 +727,175 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07AC49EF-82C2-4BDE-A85F-76318C85DA06}">
-  <dimension ref="A2:A11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B11:D11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
AR GUI dev, added laser control
</commit_message>
<xml_diff>
--- a/Script.xlsx
+++ b/Script.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Alpha Redux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2455A06A-BFE0-4616-8C39-4BFA383FB26F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E43927-B7B5-4A08-99E6-805D11193824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1875" yWindow="-19200" windowWidth="16530" windowHeight="11340" xr2:uid="{F78622BC-B8A3-4261-86B1-C19D8BE4EB55}"/>
+    <workbookView xWindow="3540" yWindow="5220" windowWidth="28800" windowHeight="15285" activeTab="1" xr2:uid="{F78622BC-B8A3-4261-86B1-C19D8BE4EB55}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="32">
   <si>
     <t>Step#</t>
   </si>
@@ -114,6 +114,24 @@
   </si>
   <si>
     <t>Wait (ms)</t>
+  </si>
+  <si>
+    <t>Reset Intlk Timer</t>
+  </si>
+  <si>
+    <t>Clears serial buffer and takes one initial (start) reading from MCU</t>
+  </si>
+  <si>
+    <t>Laser Sys ON</t>
+  </si>
+  <si>
+    <t>1 or 0</t>
+  </si>
+  <si>
+    <t>1 - ON, 0 - OFF</t>
+  </si>
+  <si>
+    <t>Laser ENA</t>
   </si>
 </sst>
 </file>
@@ -149,8 +167,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -468,20 +492,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F69CE37-DE2A-400D-95D7-88241DD5D745}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
-    <col min="3" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -498,7 +522,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
@@ -515,41 +539,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="C4">
-        <v>500</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>40</v>
       </c>
@@ -557,16 +575,16 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>300</v>
+        <v>50</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>50</v>
       </c>
@@ -574,7 +592,7 @@
         <v>13</v>
       </c>
       <c r="C6">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -583,60 +601,45 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>60</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="C7">
-        <v>5</v>
-      </c>
-      <c r="D7">
         <v>1</v>
       </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
+        <v>65</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>70</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8">
-        <v>500</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>80</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
       <c r="C9">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
@@ -651,60 +654,99 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
+        <v>90</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>100</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>110</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <v>500</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>120</v>
+      </c>
+      <c r="B14" t="s">
         <v>10</v>
       </c>
-      <c r="C11">
-        <v>20</v>
-      </c>
-      <c r="D11">
+      <c r="C14">
+        <v>30</v>
+      </c>
+      <c r="D14">
         <v>5</v>
       </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>110</v>
-      </c>
-      <c r="B12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>120</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>130</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>140</v>
+      </c>
+      <c r="B16" t="s">
         <v>11</v>
       </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D11 C13:D16 C12" xr:uid="{E060BF54-3F95-4B65-8BA7-AC011ACA6E26}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D19" xr:uid="{E060BF54-3F95-4B65-8BA7-AC011ACA6E26}">
       <formula1>0</formula1>
       <formula2>2000</formula2>
     </dataValidation>
@@ -715,9 +757,9 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" showErrorMessage="1" xr:uid="{C0A13E9A-568B-4A2B-A58D-3A0882E36B88}">
           <x14:formula1>
-            <xm:f>Sheet2!$A$2:$A$11</xm:f>
+            <xm:f>Sheet2!$A$2:$A$14</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B25</xm:sqref>
+          <xm:sqref>B2:B28</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -727,173 +769,233 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07AC49EF-82C2-4BDE-A85F-76318C85DA06}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="45.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="60" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="F11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="F12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="F13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B14:D14"/>
     <mergeCell ref="B11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>